<commit_message>
Update Excel with Variance values
</commit_message>
<xml_diff>
--- a/AccurecyChangeWithVariables.xlsx
+++ b/AccurecyChangeWithVariables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noora\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pia\Documents\IPAI_PS\IPAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407CA8B4-1011-4CF2-8132-8B5154062AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C95979-C930-4306-A96F-97EBF83B0B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{65CE57E4-A7E7-4EFB-823E-5F7F512F290A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{65CE57E4-A7E7-4EFB-823E-5F7F512F290A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="165">
   <si>
     <t>Entropy</t>
   </si>
@@ -172,6 +172,354 @@
   </si>
   <si>
     <t>DB Plus /Genuine/synthethic</t>
+  </si>
+  <si>
+    <t>Variance 003</t>
+  </si>
+  <si>
+    <t>Variance 004</t>
+  </si>
+  <si>
+    <t>Variance spoofed</t>
+  </si>
+  <si>
+    <t>DB Plus /Genuine/synthethic 003 / synthetic 004 / spoofed with knn k=3</t>
+  </si>
+  <si>
+    <t>F=10,K=5,abs</t>
+  </si>
+  <si>
+    <t>F=20,K=3,abs</t>
+  </si>
+  <si>
+    <t>F=30,K=3,abs</t>
+  </si>
+  <si>
+    <t>F=40,K=3,abs</t>
+  </si>
+  <si>
+    <t>F=50,K=3,abs</t>
+  </si>
+  <si>
+    <t>F=100,K=3,abs</t>
+  </si>
+  <si>
+    <t>F=10x10,K=3,abs</t>
+  </si>
+  <si>
+    <t>F=20x20,K=3,abs</t>
+  </si>
+  <si>
+    <t>F=30x30,K=3,abs</t>
+  </si>
+  <si>
+    <t>F=40x40,K=3,abs</t>
+  </si>
+  <si>
+    <t>F=50x50,K=3,abs</t>
+  </si>
+  <si>
+    <t>F=70x70,K=3,abs</t>
+  </si>
+  <si>
+    <t>F=100x100,K=3,abs</t>
+  </si>
+  <si>
+    <t>F=100x200,K=3,abs</t>
+  </si>
+  <si>
+    <t>55.39</t>
+  </si>
+  <si>
+    <t>72.52</t>
+  </si>
+  <si>
+    <t>77.22</t>
+  </si>
+  <si>
+    <t>78.14</t>
+  </si>
+  <si>
+    <t>78.48</t>
+  </si>
+  <si>
+    <t>76.57</t>
+  </si>
+  <si>
+    <t>78.20</t>
+  </si>
+  <si>
+    <t>75.96</t>
+  </si>
+  <si>
+    <t>83.39</t>
+  </si>
+  <si>
+    <t>85.86</t>
+  </si>
+  <si>
+    <t>86.82</t>
+  </si>
+  <si>
+    <t>87.68</t>
+  </si>
+  <si>
+    <t>89.19</t>
+  </si>
+  <si>
+    <t>88.96</t>
+  </si>
+  <si>
+    <t>79.93</t>
+  </si>
+  <si>
+    <t>79.06</t>
+  </si>
+  <si>
+    <t>78.97</t>
+  </si>
+  <si>
+    <t>81.25</t>
+  </si>
+  <si>
+    <t>81.20</t>
+  </si>
+  <si>
+    <t>80.29</t>
+  </si>
+  <si>
+    <t>81.75</t>
+  </si>
+  <si>
+    <t>80.98</t>
+  </si>
+  <si>
+    <t>66.43</t>
+  </si>
+  <si>
+    <t>64.03</t>
+  </si>
+  <si>
+    <t>65.28</t>
+  </si>
+  <si>
+    <t>68.20</t>
+  </si>
+  <si>
+    <t>66.21</t>
+  </si>
+  <si>
+    <t>64.32</t>
+  </si>
+  <si>
+    <t>63.61</t>
+  </si>
+  <si>
+    <t>71.66</t>
+  </si>
+  <si>
+    <t>76.56</t>
+  </si>
+  <si>
+    <t>76.37</t>
+  </si>
+  <si>
+    <t>76.85</t>
+  </si>
+  <si>
+    <t>75.83</t>
+  </si>
+  <si>
+    <t>71.02</t>
+  </si>
+  <si>
+    <t>73.39</t>
+  </si>
+  <si>
+    <t>64.80</t>
+  </si>
+  <si>
+    <t>62.86</t>
+  </si>
+  <si>
+    <t>65.30</t>
+  </si>
+  <si>
+    <t>67.55</t>
+  </si>
+  <si>
+    <t>68.17</t>
+  </si>
+  <si>
+    <t>67.31</t>
+  </si>
+  <si>
+    <t>66.50</t>
+  </si>
+  <si>
+    <t>DB Plus /Genuine/synthethic 003 / synthetic 004 / spoofed with knn k=5</t>
+  </si>
+  <si>
+    <t>57.52</t>
+  </si>
+  <si>
+    <t>72.43</t>
+  </si>
+  <si>
+    <t>76.53</t>
+  </si>
+  <si>
+    <t>78.29</t>
+  </si>
+  <si>
+    <t>77.49</t>
+  </si>
+  <si>
+    <t>76.31</t>
+  </si>
+  <si>
+    <t>77.46</t>
+  </si>
+  <si>
+    <t>72.72</t>
+  </si>
+  <si>
+    <t>64.86</t>
+  </si>
+  <si>
+    <t>66.30</t>
+  </si>
+  <si>
+    <t>68.03</t>
+  </si>
+  <si>
+    <t>67.68</t>
+  </si>
+  <si>
+    <t>65.92</t>
+  </si>
+  <si>
+    <t>65.44</t>
+  </si>
+  <si>
+    <t>66.91</t>
+  </si>
+  <si>
+    <t>56.38</t>
+  </si>
+  <si>
+    <t>73.85</t>
+  </si>
+  <si>
+    <t>78.54</t>
+  </si>
+  <si>
+    <t>77.93</t>
+  </si>
+  <si>
+    <t>78.94</t>
+  </si>
+  <si>
+    <t>77.74</t>
+  </si>
+  <si>
+    <t>77.28</t>
+  </si>
+  <si>
+    <t>74.50</t>
+  </si>
+  <si>
+    <t>64.06</t>
+  </si>
+  <si>
+    <t>63.57</t>
+  </si>
+  <si>
+    <t>66.81</t>
+  </si>
+  <si>
+    <t>68.08</t>
+  </si>
+  <si>
+    <t>68.82</t>
+  </si>
+  <si>
+    <t>68.51</t>
+  </si>
+  <si>
+    <t>83.94</t>
+  </si>
+  <si>
+    <t>86.04</t>
+  </si>
+  <si>
+    <t>88.32</t>
+  </si>
+  <si>
+    <t>88.87</t>
+  </si>
+  <si>
+    <t>89.14</t>
+  </si>
+  <si>
+    <t>88.69</t>
+  </si>
+  <si>
+    <t>80.43</t>
+  </si>
+  <si>
+    <t>79.52</t>
+  </si>
+  <si>
+    <t>82.25</t>
+  </si>
+  <si>
+    <t>82.53</t>
+  </si>
+  <si>
+    <t>82.48</t>
+  </si>
+  <si>
+    <t>81.89</t>
+  </si>
+  <si>
+    <t>F=20,K=5,abs</t>
+  </si>
+  <si>
+    <t>F=30,K=5,abs</t>
+  </si>
+  <si>
+    <t>F=40,K=5,abs</t>
+  </si>
+  <si>
+    <t>F=50,K=5,abs</t>
+  </si>
+  <si>
+    <t>F=100,K=5,abs</t>
+  </si>
+  <si>
+    <t>F=10x10,K=5,abs</t>
+  </si>
+  <si>
+    <t>F=20x20,K=5,abs</t>
+  </si>
+  <si>
+    <t>F=30x30,K=5,abs</t>
+  </si>
+  <si>
+    <t>F=40x40,K=5,abs</t>
+  </si>
+  <si>
+    <t>F=50x50,K=5,abs</t>
+  </si>
+  <si>
+    <t>F=70x70,K=5,abs</t>
+  </si>
+  <si>
+    <t>F=100x100,K=5,abs</t>
+  </si>
+  <si>
+    <t>F=100x200,K=5,abs</t>
   </si>
 </sst>
 </file>
@@ -331,16 +679,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -356,7 +704,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -652,53 +1000,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94451A9C-7A1C-47BA-93B3-ED88E648ADB4}">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:R42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.9453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.3671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.26171875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.62890625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.62890625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.89453125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.15625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.26171875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.15625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.734375" style="1" customWidth="1"/>
-    <col min="12" max="13" width="11.15625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.68359375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.05078125" customWidth="1"/>
-    <col min="16" max="17" width="8.83984375" style="1"/>
-    <col min="18" max="18" width="26.62890625" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="1" width="10.9296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.73046875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.59765625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.59765625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.86328125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.265625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1328125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.73046875" style="1" customWidth="1"/>
+    <col min="12" max="13" width="11.1328125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.06640625" customWidth="1"/>
+    <col min="16" max="17" width="8.86328125" style="1"/>
+    <col min="18" max="18" width="26.59765625" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.86328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.3" x14ac:dyDescent="0.7">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:18" ht="15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-    </row>
-    <row r="2" spans="1:18" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+    </row>
+    <row r="2" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -748,7 +1096,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -798,36 +1146,36 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="R4" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:18" ht="71.25" x14ac:dyDescent="0.45">
       <c r="R5" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.3" x14ac:dyDescent="0.7">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:18" ht="15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-    </row>
-    <row r="7" spans="1:18" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+    </row>
+    <row r="7" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
@@ -874,177 +1222,624 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="12">
         <v>1</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="12">
         <v>1</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="12">
         <v>1</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="12">
         <v>1</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="12">
         <v>1</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="12">
         <v>1</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="12">
         <v>1</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="12">
         <v>1</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="12">
         <v>1</v>
       </c>
-      <c r="K8" s="14">
+      <c r="K8" s="12">
         <v>1</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L8" s="12">
         <v>1</v>
       </c>
-      <c r="M8" s="14">
+      <c r="M8" s="12">
         <v>1</v>
       </c>
-      <c r="N8" s="14">
+      <c r="N8" s="12">
         <v>1</v>
       </c>
-      <c r="O8" s="14">
+      <c r="O8" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="4" t="s">
+    <row r="9" spans="1:18" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="11" spans="1:18" ht="15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+    </row>
+    <row r="12" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="O13" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="P13" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="O14" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="P14" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="O15" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="P15" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:16" ht="15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+    </row>
+    <row r="18" spans="1:16" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="M18" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="N18" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="O18" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="P18" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="O19" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="P19" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="O20" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="P20" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O21" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="P21" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O22" s="1"/>
+    </row>
+    <row r="28" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="6" t="s">
+    <row r="29" spans="1:16" ht="185.25" x14ac:dyDescent="0.45">
+      <c r="A29" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B29" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="6" t="s">
+    <row r="30" spans="1:16" ht="185.25" x14ac:dyDescent="0.45">
+      <c r="A30" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B30" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="6" t="s">
+    <row r="31" spans="1:16" ht="142.5" x14ac:dyDescent="0.45">
+      <c r="A31" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B31" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="6" t="s">
+    <row r="32" spans="1:16" ht="185.25" x14ac:dyDescent="0.45">
+      <c r="A32" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B32" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="6" t="s">
+    <row r="33" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+      <c r="A33" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B33" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="6" t="s">
+    <row r="34" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+      <c r="A34" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B34" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="6" t="s">
+    <row r="35" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+      <c r="A35" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B35" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="9" t="s">
+    <row r="36" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+      <c r="A36" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B36" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="9" t="s">
+    <row r="37" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+      <c r="A37" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B37" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="9" t="s">
+    <row r="38" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+      <c r="A38" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B38" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="9" t="s">
+    <row r="39" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+      <c r="A39" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B39" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="9" t="s">
+    <row r="40" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+      <c r="A40" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B40" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="9" t="s">
+    <row r="41" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+      <c r="A41" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B41" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="9" t="s">
+    <row r="42" spans="1:2" ht="185.25" x14ac:dyDescent="0.45">
+      <c r="A42" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B42" s="10" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="A6:O6"/>
+    <mergeCell ref="A11:O11"/>
+    <mergeCell ref="A17:O17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>